<commit_message>
Creados procedimientos para la lectura de excel de equipos y campos
</commit_message>
<xml_diff>
--- a/Equipos.xlsx
+++ b/Equipos.xlsx
@@ -39,9 +39,6 @@
     <t>A.C. Plataneiras F7</t>
   </si>
   <si>
-    <t>Tratagua's Team</t>
-  </si>
-  <si>
     <t>Suso NT Grupo Parranda F7</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>Af. LagunaGest Asesores F7</t>
   </si>
   <si>
-    <t>Liga Veteranos+30</t>
-  </si>
-  <si>
     <t>Sin división</t>
   </si>
   <si>
@@ -270,9 +264,6 @@
     <t>San Cristóbal F7 Veteranos</t>
   </si>
   <si>
-    <t>Valleseco Vet. "B" F7</t>
-  </si>
-  <si>
     <t>Once Diablos F7 Vet.+35</t>
   </si>
   <si>
@@ -298,6 +289,15 @@
   </si>
   <si>
     <t>Servicio Técnico Los Reyes</t>
+  </si>
+  <si>
+    <t>Trataguas Team</t>
+  </si>
+  <si>
+    <t>Liga Veteranos +30</t>
+  </si>
+  <si>
+    <t>Valleseco Vet. B F7</t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,7 @@
   <dimension ref="A1:C85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C85"/>
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -691,7 +691,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -713,7 +713,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -812,7 +812,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -823,505 +823,505 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
         <v>34</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" t="s">
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
         <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B43" t="s">
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
@@ -1329,10 +1329,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -1340,10 +1340,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
@@ -1351,10 +1351,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
@@ -1362,10 +1362,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
@@ -1373,10 +1373,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
@@ -1384,10 +1384,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
@@ -1395,10 +1395,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C69" t="s">
         <v>5</v>
@@ -1417,10 +1417,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
@@ -1428,10 +1428,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
@@ -1439,10 +1439,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C72" t="s">
         <v>5</v>
@@ -1450,145 +1450,145 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C73" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C74" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C75" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="3" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B76" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C76" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B77" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C77" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B78" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C78" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B79" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C79" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B80" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C80" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B81" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C81" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B82" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C82" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B83" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C83" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C84" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B85" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C85" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pruebas para cargar datos de calendario nuevamente
</commit_message>
<xml_diff>
--- a/Equipos.xlsx
+++ b/Equipos.xlsx
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>